<commit_message>
Add more background figures and data visualizations on ACE2 seqs and RBD ASR/phylogeny
</commit_message>
<xml_diff>
--- a/RBD_ASR/parsed_sequences/RBD_sequence_set.xlsx
+++ b/RBD_ASR/parsed_sequences/RBD_sequence_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstarr/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstarr/Desktop/RBD_ASR/parsed_sequences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4A8A8F-79CB-444E-9573-0DF94F3AD8C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F84B60-AF2A-D74D-83F0-557D181E8995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28980" yWindow="-420" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21380" yWindow="460" windowWidth="21320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBD_sequence_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="371">
   <si>
     <t>AncSarbecovirus_MAP</t>
   </si>
@@ -1137,6 +1137,12 @@
   </si>
   <si>
     <t>G138</t>
+  </si>
+  <si>
+    <t>F-&gt;T</t>
+  </si>
+  <si>
+    <t>V170</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1291,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1483,6 +1489,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1644,13 +1656,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2010,7 +2023,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
+      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3849,11 +3862,29 @@
       <c r="B52" t="s">
         <v>92</v>
       </c>
-      <c r="C52" t="s">
-        <v>278</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>142</v>
+      <c r="C52" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="F52" t="s">
+        <v>162</v>
+      </c>
+      <c r="G52" t="s">
+        <v>168</v>
+      </c>
+      <c r="H52" t="s">
+        <v>174</v>
+      </c>
+      <c r="I52" t="s">
+        <v>180</v>
+      </c>
+      <c r="J52" t="s">
+        <v>284</v>
+      </c>
+      <c r="K52" t="s">
+        <v>370</v>
       </c>
       <c r="L52" t="s">
         <v>345</v>

</xml_diff>

<commit_message>
add new isogenic plasmid designs
</commit_message>
<xml_diff>
--- a/RBD_ASR/parsed_sequences/RBD_sequence_set.xlsx
+++ b/RBD_ASR/parsed_sequences/RBD_sequence_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstarr/Desktop/RBD_ASR/parsed_sequences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F84B60-AF2A-D74D-83F0-557D181E8995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB78B58B-BB0C-3A4D-8EEA-033AEA6BF6C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21380" yWindow="460" windowWidth="21320" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4040" yWindow="720" windowWidth="25640" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBD_sequence_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="430">
   <si>
     <t>AncSarbecovirus_MAP</t>
   </si>
@@ -1143,6 +1143,183 @@
   </si>
   <si>
     <t>V170</t>
+  </si>
+  <si>
+    <t>Rc-o319_LC556375</t>
+  </si>
+  <si>
+    <t>NITNLCPFSEVFNATTFASVYAWNRKRISNCVADYSVLYNST-SFSTFQCYGVSSTKLNDLCFTNVYADSFVVRGDEVRQIAPGQTGVIADYNYKLPDDFTGCVLAWNSRNQDASTSGNFNYYYRIWRSEKLRPFERDIAHYDYQVGTQFKSS---------LKNYGFYSSAGDSHQPYRVVVLSFELLNAPATVCGPKQST</t>
+  </si>
+  <si>
+    <t>RshSTT182_EPI_ISL_852604</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFASVYAWNRRRISNCVADYSVLYNTT-SFSTFKCYGVSPTKLNDLCFTNVYADSFVVRGDEVRQIAPGQTGKIADYNYKLPDDFMGCVIAWNSISLDA--GGS--YYYRLFRKSVLKPFERDISTQLYQAGDKPCS-VEGPDCYYPLQSYYFQSTNGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>RacCS203_MW251308</t>
+  </si>
+  <si>
+    <t>NITNFCPFDKVFNATRFPNVYAWQRTKISDCIADYTVLYNST-SFSTFKCYGVSPSKLIDLCFTSVYADTFLIRFSEVRQIAPGETGVIADYNYKLPDDFTGCVLAWNTAKQDIGS-----YFYRSHRAVKLKPFERDLSSDE--------------NGVRTLSTYDFNPNVPLDYQATRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGQVFNASKFPSVYAWERLRISDCVADYSVLYNSSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSVDSKQ--GNNFYYRLFRHGKIKPYERDISNVLYNSAGGTCSSTSQLGCYEPLKSYGFTPTVGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>PRD-0038_726045</t>
+  </si>
+  <si>
+    <t>PDF-2370_MT726044</t>
+  </si>
+  <si>
+    <t>NITNLCPFGQVFNASNFPSVYAWERLRISDCVADYSVLYNSSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSVDSKQ--G-NFYYRLFRHGKIKPYERDISNVLYNSAGGTCSSISQLGCYEPLKSYGFTPTVGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>AncSarbecovirus_GARD</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFPSVYAWERMRISNCVADYSVLYNSS-SFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSS--GNNFFYRLFRHGKIKPYERDISNVLYNPAGGTCSSISGLNCYKPLKSYGFTPTSGVGYQPYRVVVLSFELLNAPATVCGPKQST</t>
+  </si>
+  <si>
+    <t>AncSarbecovirus_GARD+K493Y</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFPSVYAWERMRISNCVADYSVLYNSS-SFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSS--GNNFFYRLFRHGKIKPYERDISNVLYNPAGGTCSSISGLNCYKPLYSYGFTPTSGVGYQPYRVVVLSFELLNAPATVCGPKQST</t>
+  </si>
+  <si>
+    <t>AncAsia_GARD</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFPSVYAWERKRISNCVADYSVLYNST-SFSTFKCYGVSPTKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSTSGNYNYLYRLFRHGKLKPYERDISNVIYSPGGQSCS-AVGLNCYNPLKSYGFYTTSGVGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>SARS2+Q498Y</t>
+  </si>
+  <si>
+    <t>SARS2+N501Y</t>
+  </si>
+  <si>
+    <t>SARS2+Q498Y+N501Y</t>
+  </si>
+  <si>
+    <t>SARS1+Y498Q</t>
+  </si>
+  <si>
+    <t>SARS1+T501Y</t>
+  </si>
+  <si>
+    <t>SARS1+Y498Q+T501Y</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSA-SFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTNGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSA-SFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFQPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSA-SFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNST-FFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCT-PPALNCYWPLNDYGFQTTTGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNST-FFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCT-PPALNCYWPLNDYGFYTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNST-FFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCT-PPALNCYWPLNDYGFQTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>PRD-0038+K493Y+T498W</t>
+  </si>
+  <si>
+    <t>NITNLCPFGQVFNASKFPSVYAWERLRISDCVADYSVLYNSSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSVDSKQ--GNNFYYRLFRHGKIKPYERDISNVLYNSAGGTCSSTSQLGCYEPLYSYGFWPTVGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFSEVFNATTFASVYAWNRKRISNCVADYSVLYNSTSFSTFQCYGVSSTKLNDLCFTNVYADSFVVRGDEVRQIAPGQTGVIADYNYKLPDDFTGCVLAWNSRNQDASTSGNFNYYYRIWRSEKLRPFERDIAHYDYQVGTQFKSSLKNYGFYSSAGDSHQPYRVVVLSFELLNAPATVCGPKQST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFASVYAWNRRRISNCVADYSVLYNTTSFSTFKCYGVSPTKLNDLCFTNVYADSFVVRGDEVRQIAPGQTGKIADYNYKLPDDFMGCVIAWNSISLDAGGSYYYRLFRKSVLKPFERDISTQLYQAGDKPCSVEGPDCYYPLQSYYFQSTNGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNFCPFDKVFNATRFPNVYAWQRTKISDCIADYTVLYNSTSFSTFKCYGVSPSKLIDLCFTSVYADTFLIRFSEVRQIAPGETGVIADYNYKLPDDFTGCVLAWNTAKQDIGSYFYRSHRAVKLKPFERDLSSDENGVRTLSTYDFNPNVPLDYQATRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGQVFNASKFPSVYAWERLRISDCVADYSVLYNSSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSVDSKQGNNFYYRLFRHGKIKPYERDISNVLYNSAGGTCSSTSQLGCYEPLKSYGFTPTVGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGQVFNASNFPSVYAWERLRISDCVADYSVLYNSSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSVDSKQGNFYYRLFRHGKIKPYERDISNVLYNSAGGTCSSISQLGCYEPLKSYGFTPTVGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGQVFNASKFPSVYAWERLRISDCVADYSVLYNSSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSVDSKQGNNFYYRLFRHGKIKPYERDISNVLYNSAGGTCSSTSQLGCYEPLYSYGFWPTVGVGYQPYRVVVLSFELLNAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFPSVYAWERMRISNCVADYSVLYNSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSSGNNFFYRLFRHGKIKPYERDISNVLYNPAGGTCSSISGLNCYKPLKSYGFTPTSGVGYQPYRVVVLSFELLNAPATVCGPKQST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFPSVYAWERMRISNCVADYSVLYNSSSFSTFKCYGVSPTKLNDLCFSSVYADYFVVKGDDVRQIAPAQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSSGNNFFYRLFRHGKIKPYERDISNVLYNPAGGTCSSISGLNCYKPLYSYGFTPTSGVGYQPYRVVVLSFELLNAPATVCGPKQST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATTFPSVYAWERKRISNCVADYSVLYNSTSFSTFKCYGVSPTKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSTSGNYNYLYRLFRHGKLKPYERDISNVIYSPGGQSCSAVGLNCYNPLKSYGFYTTSGVGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSASFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTNGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSASFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFQPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSASFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNSTFFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCTPPALNCYWPLNDYGFQTTTGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNSTFFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCTPPALNCYWPLNDYGFYTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNSTFFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCTPPALNCYWPLNDYGFQTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
+  </si>
+  <si>
+    <t>AACATTACAAATCTATGTCCCTTCTCCGAGGTATTTAACGCTACCACATTCGCTAGTGTGTATGCTTGGAACAGGAAGCGTATTTCTAATTGTGTTGCCGATTACTCAGTCTTATACAACAGTACCTCATTCTCTACTTTTCAGTGTTATGGAGTCTCTTCTACAAAGCTTAACGACCTGTGCTTCACCAATGTGTACGCCGATTCCTTTGTTGTCAGGGGGGATGAGGTGCGTCAGATAGCACCAGGCCAAACGGGCGTTATAGCGGACTACAACTATAAGTTACCAGACGATTTTACCGGATGCGTCTTGGCGTGGAATTCAAGAAACCAAGACGCGAGTACCTCCGGGAACTTTAATTACTATTATCGTATCTGGAGAAGTGAAAAACTTCGTCCCTTTGAGAGGGACATCGCTCACTATGACTATCAAGTAGGGACCCAGTTTAAGTCTTCTCTTAAGAATTATGGATTCTATTCCAGCGCAGGGGACTCTCATCAACCGTACAGAGTAGTCGTACTAAGTTTCGAGTTATTGAACGCGCCTGCCACCGTTTGCGGTCCCAAACAGTCAACA</t>
+  </si>
+  <si>
+    <t>AATATCACAAATCTGTGCCCATTCGGAGAGGTTTTCAATGCGACCACTTTTGCTAGCGTGTATGCTTGGAATAGGCGTAGGATTTCAAATTGTGTGGCTGATTACAGCGTCTTGTATAATACGACTTCCTTCAGCACTTTTAAATGTTACGGCGTCAGTCCCACAAAACTTAACGACCTGTGTTTCACAAATGTTTATGCGGACTCATTCGTGGTTCGTGGCGACGAAGTGAGACAGATAGCCCCAGGGCAGACCGGGAAAATAGCTGACTATAATTATAAATTACCAGACGATTTCATGGGATGCGTTATAGCGTGGAACTCAATCTCTTTAGACGCAGGAGGAAGCTACTACTACAGGTTATTTAGGAAGAGTGTACTTAAACCATTCGAGAGGGACATTTCTACGCAGCTATACCAAGCTGGGGACAAACCTTGCAGCGTGGAAGGACCAGACTGCTATTATCCGTTGCAGAGTTATTACTTTCAAAGCACAAACGGGGTCGGATACCAACCTTATAGGGTTGTCGTACTATCATTTGAGCTGTTAAACGCCCCGGCGACAGTATGTGGGCCTAAGAAGTCAACG</t>
+  </si>
+  <si>
+    <t>AATATCACCAATCTTTGTCCCTTCGGTCAAGTGTTTAACGCATCTAAGTTCCCCAGTGTGTATGCTTGGGAAAGGTTACGTATTAGCGATTGCGTGGCCGATTATTCCGTCCTGTATAATAGCAGTTCATCCTTCTCAACCTTTAAGTGTTACGGCGTTTCTCCAACTAAGTTAAACGATTTATGTTTCAGTTCCGTTTACGCTGACTACTTTGTGGTCAAAGGGGACGACGTAAGGCAAATAGCCCCTGCCCAGACTGGGGTAATAGCTGATTATAACTACAAGCTTCCCGACGATTTCACCGGATGTGTCTTGGCTTGGAACACTAACTCAGTGGACAGTAAGCAGGGGAATAATTTTTATTATCGTCTTTTTCGTCACGGCAAGATTAAGCCTTACGAAAGGGATATTAGCAACGTCCTTTATAATAGCGCGGGTGGCACTTGCTCTAGTACATCACAGCTAGGATGCTACGAGCCATTGAAGTCTTACGGGTTCACACCCACTGTAGGCGTGGGCTACCAGCCGTACCGTGTGGTCGTCCTTAGCTTTGAGTTATTGAACGCCCCAGCCACCGTTTGTGGACCAAAAAAGTCTACG</t>
+  </si>
+  <si>
+    <t>AACATTACGAATTTGTGTCCGTTCGGTCAGGTTTTCAATGCCTCAAACTTTCCGTCTGTCTACGCATGGGAAAGATTGCGTATCTCCGATTGTGTCGCCGACTACTCTGTTCTGTACAATAGCAGCTCATCCTTCAGTACGTTTAAGTGTTACGGGGTTTCTCCAACAAAACTAAATGACTTGTGCTTTAGTTCCGTATATGCGGACTATTTTGTCGTGAAAGGCGACGATGTAAGACAGATAGCCCCTGCTCAGACAGGTGTAATAGCCGATTACAACTACAAGCTGCCCGACGACTTTACCGGTTGTGTCCTGGCATGGAATACCAATTCAGTCGATTCCAAGCAAGGCAATTTCTATTACAGGTTATTTAGACACGGAAAGATTAAGCCTTATGAGAGAGACATATCAAACGTCTTATATAACAGCGCTGGAGGCACCTGTTCATCCATTTCCCAGCTTGGCTGTTACGAACCTTTGAAATCTTATGGTTTTACGCCCACTGTAGGTGTTGGGTACCAGCCGTACCGTGTTGTAGTCTTATCTTTCGAGTTACTGAACGCTCCTGCGACCGTTTGCGGACCTAAAAAGAGCACT</t>
+  </si>
+  <si>
+    <t>AACATAACGAACTTATGCCCCTTTGGTCAGGTTTTCAATGCTAGCAAGTTTCCCTCAGTTTACGCTTGGGAAAGGCTAAGGATCAGCGACTGTGTCGCAGACTACAGTGTTCTTTACAATTCTAGCTCCTCTTTCTCCACGTTCAAATGTTATGGGGTTTCACCAACGAAACTAAATGACTTGTGCTTTTCCTCCGTGTATGCCGATTATTTCGTAGTGAAGGGTGACGATGTAAGGCAGATAGCCCCGGCGCAAACAGGTGTTATAGCTGATTACAATTATAAATTACCCGATGACTTTACAGGATGCGTGCTAGCCTGGAATACTAACTCCGTAGATTCAAAACAAGGGAACAACTTTTACTACAGATTGTTTCGTCATGGCAAAATCAAACCTTATGAAAGGGATATTAGCAATGTGTTATACAACAGCGCCGGAGGCACTTGCAGCTCCACGTCTCAATTAGGATGTTATGAGCCCTTATATTCTTATGGCTTTTGGCCCACCGTTGGTGTTGGATACCAGCCATATAGGGTAGTAGTCTTGTCTTTTGAATTGTTGAACGCTCCAGCTACGGTGTGCGGCCCAAAGAAATCAACC</t>
+  </si>
+  <si>
+    <t>AACATCACAAATCTTTGCCCGTTTGGCGAAGTATTTAATGCGACTACGTTTCCTTCCGTGTACGCGTGGGAGAGGATGAGGATTTCTAACTGTGTGGCTGATTACAGCGTGCTATACAACTCATCTAGTTTCAGCACTTTCAAGTGTTACGGGGTTTCTCCCACTAAGCTGAACGACCTTTGTTTCTCAAGCGTTTACGCTGACTATTTTGTTGTAAAAGGGGACGACGTTAGACAGATTGCACCCGCGCAAACGGGGGTAATAGCAGACTATAATTACAAACTACCCGACGACTTCACTGGTTGTGTATTGGCCTGGAACACAAACTCCCTGGACAGTAGCTCAGGAAACAACTTTTTTTATAGGTTATTTAGACATGGTAAAATTAAACCGTATGAACGTGACATATCTAACGTACTTTATAATCCCGCGGGTGGAACATGCAGCTCTATCAGTGGCCTTAACTGCTACAAACCGCTAAAATCCTATGGGTTTACCCCTACGAGCGGGGTCGGGTATCAGCCGTACCGTGTCGTGGTGCTTTCATTTGAACTATTAAACGCCCCGGCAACCGTGTGCGGTCCTAAGCAAAGCACA</t>
+  </si>
+  <si>
+    <t>AACATTACAAACTTGTGCCCCTTCGGAGAGGTCTTTAACGCAACTACGTTTCCAAGTGTGTACGCCTGGGAAAGGATGAGGATATCAAATTGTGTTGCGGATTACAGCGTCTTGTATAACTCATCCAGCTTTTCCACCTTTAAATGTTATGGGGTCAGCCCTACTAAGTTGAATGACTTATGTTTCTCCAGCGTTTATGCAGATTACTTTGTCGTGAAGGGGGACGATGTACGTCAGATCGCCCCTGCACAAACCGGGGTTATAGCTGACTACAATTACAAACTTCCTGACGATTTCACTGGTTGCGTATTAGCGTGGAACACTAACAGCCTAGATTCAAGCAGTGGGAACAATTTTTTTTATAGATTGTTTAGACATGGAAAGATCAAACCTTATGAGAGGGATATCAGTAATGTCCTATATAACCCCGCAGGTGGCACTTGCTCCAGCATCTCCGGGCTAAATTGTTACAAGCCACTTTACAGCTATGGCTTTACTCCTACCTCCGGGGTCGGCTATCAGCCATATAGGGTAGTGGTACTGAGTTTTGAATTACTGAACGCACCCGCTACTGTTTGTGGCCCGAAACAGTCTACG</t>
+  </si>
+  <si>
+    <t>AATATCACAAATTTGTGCCCGTTCGGAGAGGTTTTTAACGCTACCACGTTTCCTAGTGTTTACGCCTGGGAGAGGAAGAGAATTAGCAATTGTGTAGCCGATTACTCTGTGCTATACAACAGTACATCCTTTTCAACCTTCAAATGCTATGGTGTTAGCCCAACAAAACTGAACGATTTATGCTTCTCTAATGTCTATGCAGATTCTTTCGTGGTGAAAGGGGATGATGTTCGTCAAATCGCGCCGGGTCAAACTGGTGTGATAGCGGACTATAATTACAAGTTGCCGGATGATTTCACTGGTTGTGTTTTAGCATGGAACACGAACTCATTAGATTCCTCTACAAGCGGCAACTACAATTATCTGTATAGGTTATTCAGACACGGGAAACTGAAGCCGTATGAGAGGGACATCTCTAACGTCATCTACAGTCCTGGTGGACAATCATGTTCAGCCGTCGGGCTAAATTGTTACAATCCCCTGAAAAGCTATGGTTTCTATACAACAAGCGGTGTGGGCTATCAGCCCTACCGTGTTGTTGTCCTGTCCTTCGAATTATTAAATGCCCCTGCAACTGTATGCGGGCCTAAGCTATCCACG</t>
+  </si>
+  <si>
+    <t>AACATCACAAACCTATGTCCGTTTGGCGAGGTGTTTAATGCTACTAGGTTCGCAAGCGTTTACGCATGGAACCGTAAGAGAATCTCTAACTGCGTCGCAGATTATAGCGTTTTATATAACTCTGCTAGTTTTTCTACTTTTAAGTGTTACGGCGTGAGTCCTACGAAGTTGAACGATCTTTGCTTTACGAATGTGTACGCGGACAGCTTTGTCATCAGAGGTGATGAGGTAAGGCAGATAGCGCCCGGACAAACGGGGAAGATCGCAGACTACAATTATAAGCTGCCAGATGACTTTACCGGATGTGTGATTGCCTGGAACTCAAATAATCTGGACTCAAAGGTGGGTGGCAACTATAACTACCTGTATCGTCTTTTTAGGAAATCAAACTTAAAACCGTTTGAAAGGGACATATCCACTGAAATATATCAAGCGGGGAGCACACCGTGCAATGGCGTCGAGGGGTTTAACTGCTATTTCCCTCTACAGTCCTATGGGTTCTATCCTACTAATGGAGTTGGTTACCAACCCTATAGAGTGGTTGTTCTTAGTTTCGAGCTACTACATGCGCCAGCGACTGTGTGCGGCCCTAAGAAATCTACG</t>
+  </si>
+  <si>
+    <t>AATATCACGAACCTGTGTCCTTTTGGGGAGGTATTTAACGCCACCCGTTTCGCTTCAGTGTATGCCTGGAATAGAAAACGTATCAGCAATTGTGTCGCAGATTATTCAGTGCTATATAACTCCGCTAGTTTCTCTACGTTTAAGTGTTATGGCGTGTCCCCAACCAAGCTGAACGACCTGTGCTTTACAAACGTATATGCGGATTCATTTGTGATTAGAGGCGATGAAGTGAGACAAATTGCCCCAGGCCAGACCGGAAAGATTGCCGACTATAATTACAAACTGCCAGACGACTTTACGGGGTGTGTCATCGCTTGGAACAGCAACAATCTTGACAGTAAAGTTGGCGGGAACTATAATTATCTGTACCGTCTGTTCAGAAAAAGTAATCTTAAACCGTTTGAAAGGGACATCAGTACTGAGATTTATCAAGCGGGCTCAACCCCGTGTAATGGTGTAGAGGGGTTTAACTGCTATTTTCCACTACAATCCTACGGCTTCCAGCCAACGTACGGTGTGGGTTATCAACCCTATCGTGTCGTCGTATTGTCCTTCGAGCTATTACATGCTCCCGCGACCGTCTGTGGACCAAAGAAGTCCACC</t>
+  </si>
+  <si>
+    <t>AATATAACCAATCTGTGTCCCTTTGGAGAGGTTTTTAACGCTACGAGGTTCGCTTCTGTATATGCCTGGAACCGTAAGAGAATATCCAACTGTGTCGCTGACTACTCAGTTCTGTACAATTCTGCTAGTTTTAGCACCTTCAAGTGCTACGGAGTCAGCCCGACGAAGCTGAACGATTTGTGTTTTACGAATGTCTACGCTGACTCCTTCGTTATCAGGGGGGACGAAGTGAGGCAAATTGCTCCTGGCCAGACAGGGAAAATTGCTGATTATAATTACAAGTTACCGGATGATTTCACTGGATGCGTTATTGCATGGAACTCTAATAACCTTGATAGTAAGGTTGGCGGCAATTACAACTATTTGTACAGATTGTTCCGTAAGTCCAACCTGAAACCCTTCGAGAGAGATATTTCAACCGAAATTTACCAGGCAGGGTCCACGCCCTGCAATGGTGTAGAAGGGTTTAATTGCTATTTCCCGTTGCAGAGCTACGGATTCTACCCAACGTATGGAGTGGGTTATCAACCTTATCGTGTTGTCGTTTTGAGCTTTGAGCTGCTACATGCACCAGCAACTGTATGCGGGCCCAAGAAGTCTACT</t>
+  </si>
+  <si>
+    <t>AACATAACAAATTTGTGCCCTTTTGGAGAAGTTTTTAATGCAACAAAATTTCCATCCGTTTACGCATGGGAAAGAAAGAAAATCAGCAATTGTGTAGCCGATTACTCAGTACTTTACAATAGCACATTCTTTAGTACTTTCAAATGTTACGGGGTTTCAGCAACGAAATTAAACGATTTATGTTTCAGTAATGTGTATGCCGATAGTTTCGTCGTCAAAGGAGATGATGTGAGACAGATTGCACCCGGCCAGACTGGAGTTATTGCAGACTATAACTACAAACTACCAGACGATTTTATGGGATGTGTATTGGCATGGAACACGAGAAACATTGATGCTACGTCTACGGGTAACTATAACTATAAATATAGATACCTTAGGCACGGGAAGTTACGTCCGTTCGAGAGAGATATATCCAATGTACCATTTAGTCCTGATGGCAAGCCTTGCACTCCACCGGCCCTGAACTGTTATTGGCCCTTGAACGATTATGGTTTTCAAACAACTACGGGCATAGGTTACCAGCCATATAGGGTGGTAGTCCTGTCATTTGAGTTATTGAATGCGCCCGCTACGGTTTGCGGACCCAAACTGTCCACG</t>
+  </si>
+  <si>
+    <t>AATATAACAAACCTGTGTCCGTTTGGAGAAGTATTCAATGCTACTAAGTTCCCATCAGTTTACGCGTGGGAAAGGAAGAAGATTAGCAACTGTGTGGCAGACTACTCAGTGCTTTACAATAGCACCTTTTTCAGTACTTTCAAGTGCTATGGAGTAAGCGCCACTAAATTGAATGATTTATGTTTCTCAAACGTTTACGCAGATTCATTCGTGGTCAAAGGTGATGACGTGCGTCAGATAGCGCCAGGACAGACAGGAGTGATAGCGGACTATAACTACAAATTGCCGGACGATTTTATGGGCTGCGTCCTGGCATGGAATACGAGGAATATTGATGCAACCTCCACTGGCAACTATAACTATAAGTATCGTTACCTGAGGCACGGGAAACTAAGACCTTTCGAGAGAGACATATCAAATGTTCCATTTAGTCCAGACGGAAAGCCATGCACACCGCCAGCCCTTAACTGTTACTGGCCTCTAAATGACTATGGCTTTTATACAACGTATGGCATTGGTTATCAGCCGTACAGGGTAGTGGTCCTTAGCTTTGAGCTATTAAACGCTCCGGCTACGGTTTGCGGACCGAAACTGTCTACT</t>
+  </si>
+  <si>
+    <t>AATATCACCAACCTGTGTCCCTTCGGCGAGGTTTTCAACGCTACAAAATTCCCCTCCGTATATGCTTGGGAGAGAAAGAAGATCAGTAATTGCGTCGCAGACTATAGTGTTCTATATAATTCCACCTTCTTTAGCACTTTTAAGTGTTATGGAGTAAGTGCTACCAAACTTAATGATCTATGTTTCTCTAACGTGTACGCCGATTCTTTCGTTGTGAAAGGTGATGATGTTCGTCAGATTGCTCCTGGGCAAACGGGAGTGATTGCAGACTACAACTATAAGCTGCCGGACGATTTCATGGGCTGTGTATTAGCTTGGAATACCAGAAATATCGACGCCACATCAACTGGCAACTACAACTACAAATACAGATACTTACGTCATGGTAAACTGCGTCCTTTTGAGAGGGACATATCTAATGTGCCATTTTCTCCAGATGGAAAGCCCTGCACTCCGCCCGCGTTAAATTGCTATTGGCCACTTAACGACTACGGATTCCAGACAACGTACGGAATTGGCTATCAGCCGTATAGGGTGGTAGTGCTGAGCTTTGAGTTGTTAAATGCGCCTGCGACAGTGTGTGGGCCGAAATTAAGTACA</t>
   </si>
 </sst>
 </file>
@@ -2019,11 +2196,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4565,6 +4742,390 @@
         <v>276</v>
       </c>
     </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>371</v>
+      </c>
+      <c r="C77">
+        <v>3001</v>
+      </c>
+      <c r="L77" t="s">
+        <v>416</v>
+      </c>
+      <c r="M77" t="s">
+        <v>401</v>
+      </c>
+      <c r="N77" t="s">
+        <v>372</v>
+      </c>
+      <c r="O77" t="s">
+        <v>275</v>
+      </c>
+      <c r="P77" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78" t="s">
+        <v>373</v>
+      </c>
+      <c r="C78">
+        <v>3002</v>
+      </c>
+      <c r="L78" t="s">
+        <v>417</v>
+      </c>
+      <c r="M78" t="s">
+        <v>402</v>
+      </c>
+      <c r="N78" t="s">
+        <v>374</v>
+      </c>
+      <c r="O78" t="s">
+        <v>275</v>
+      </c>
+      <c r="P78" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79" t="s">
+        <v>375</v>
+      </c>
+      <c r="M79" t="s">
+        <v>403</v>
+      </c>
+      <c r="N79" t="s">
+        <v>376</v>
+      </c>
+      <c r="O79" t="s">
+        <v>275</v>
+      </c>
+      <c r="P79" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80" t="s">
+        <v>378</v>
+      </c>
+      <c r="C80">
+        <v>3003</v>
+      </c>
+      <c r="L80" t="s">
+        <v>418</v>
+      </c>
+      <c r="M80" t="s">
+        <v>404</v>
+      </c>
+      <c r="N80" t="s">
+        <v>377</v>
+      </c>
+      <c r="O80" t="s">
+        <v>275</v>
+      </c>
+      <c r="P80" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81" t="s">
+        <v>379</v>
+      </c>
+      <c r="C81">
+        <v>3004</v>
+      </c>
+      <c r="L81" t="s">
+        <v>419</v>
+      </c>
+      <c r="M81" t="s">
+        <v>405</v>
+      </c>
+      <c r="N81" t="s">
+        <v>380</v>
+      </c>
+      <c r="O81" t="s">
+        <v>275</v>
+      </c>
+      <c r="P81" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82" t="s">
+        <v>399</v>
+      </c>
+      <c r="C82">
+        <v>3005</v>
+      </c>
+      <c r="L82" t="s">
+        <v>420</v>
+      </c>
+      <c r="M82" t="s">
+        <v>406</v>
+      </c>
+      <c r="N82" t="s">
+        <v>400</v>
+      </c>
+      <c r="O82" t="s">
+        <v>275</v>
+      </c>
+      <c r="P82" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83" t="s">
+        <v>381</v>
+      </c>
+      <c r="C83">
+        <v>3006</v>
+      </c>
+      <c r="L83" t="s">
+        <v>421</v>
+      </c>
+      <c r="M83" t="s">
+        <v>407</v>
+      </c>
+      <c r="N83" t="s">
+        <v>382</v>
+      </c>
+      <c r="O83" t="s">
+        <v>275</v>
+      </c>
+      <c r="P83" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84" t="s">
+        <v>383</v>
+      </c>
+      <c r="C84">
+        <v>3007</v>
+      </c>
+      <c r="L84" t="s">
+        <v>422</v>
+      </c>
+      <c r="M84" t="s">
+        <v>408</v>
+      </c>
+      <c r="N84" t="s">
+        <v>384</v>
+      </c>
+      <c r="O84" t="s">
+        <v>275</v>
+      </c>
+      <c r="P84" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85" t="s">
+        <v>385</v>
+      </c>
+      <c r="C85">
+        <v>3008</v>
+      </c>
+      <c r="L85" t="s">
+        <v>423</v>
+      </c>
+      <c r="M85" t="s">
+        <v>409</v>
+      </c>
+      <c r="N85" t="s">
+        <v>386</v>
+      </c>
+      <c r="O85" t="s">
+        <v>275</v>
+      </c>
+      <c r="P85" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86" t="s">
+        <v>387</v>
+      </c>
+      <c r="C86">
+        <v>3009</v>
+      </c>
+      <c r="L86" t="s">
+        <v>424</v>
+      </c>
+      <c r="M86" t="s">
+        <v>410</v>
+      </c>
+      <c r="N86" t="s">
+        <v>393</v>
+      </c>
+      <c r="O86" t="s">
+        <v>275</v>
+      </c>
+      <c r="P86" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87" t="s">
+        <v>388</v>
+      </c>
+      <c r="C87">
+        <v>3010</v>
+      </c>
+      <c r="L87" t="s">
+        <v>425</v>
+      </c>
+      <c r="M87" t="s">
+        <v>411</v>
+      </c>
+      <c r="N87" t="s">
+        <v>394</v>
+      </c>
+      <c r="O87" t="s">
+        <v>275</v>
+      </c>
+      <c r="P87" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>82</v>
+      </c>
+      <c r="B88" t="s">
+        <v>389</v>
+      </c>
+      <c r="C88">
+        <v>3011</v>
+      </c>
+      <c r="L88" t="s">
+        <v>426</v>
+      </c>
+      <c r="M88" t="s">
+        <v>412</v>
+      </c>
+      <c r="N88" t="s">
+        <v>395</v>
+      </c>
+      <c r="O88" t="s">
+        <v>275</v>
+      </c>
+      <c r="P88" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89" t="s">
+        <v>390</v>
+      </c>
+      <c r="C89">
+        <v>3012</v>
+      </c>
+      <c r="L89" t="s">
+        <v>427</v>
+      </c>
+      <c r="M89" t="s">
+        <v>413</v>
+      </c>
+      <c r="N89" t="s">
+        <v>396</v>
+      </c>
+      <c r="O89" t="s">
+        <v>275</v>
+      </c>
+      <c r="P89" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90" t="s">
+        <v>391</v>
+      </c>
+      <c r="C90">
+        <v>3013</v>
+      </c>
+      <c r="L90" t="s">
+        <v>428</v>
+      </c>
+      <c r="M90" t="s">
+        <v>414</v>
+      </c>
+      <c r="N90" t="s">
+        <v>397</v>
+      </c>
+      <c r="O90" t="s">
+        <v>275</v>
+      </c>
+      <c r="P90" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91" t="s">
+        <v>392</v>
+      </c>
+      <c r="C91">
+        <v>3014</v>
+      </c>
+      <c r="L91" t="s">
+        <v>429</v>
+      </c>
+      <c r="M91" t="s">
+        <v>415</v>
+      </c>
+      <c r="N91" t="s">
+        <v>398</v>
+      </c>
+      <c r="O91" t="s">
+        <v>275</v>
+      </c>
+      <c r="P91" t="s">
+        <v>276</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
remove custom annotated pdfs and ppts
</commit_message>
<xml_diff>
--- a/RBD_ASR/parsed_sequences/RBD_sequence_set.xlsx
+++ b/RBD_ASR/parsed_sequences/RBD_sequence_set.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstarr/Desktop/RBD_ASR/parsed_sequences/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/homes/bloom_j/computational_notebooks/tstarr/2020/SARSr-CoV_homolog_survey/RBD_ASR/parsed_sequences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E34779-693F-DC49-BDCE-52B32886DF04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC728DD-E862-D84C-9E50-3ACC1233364E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="720" windowWidth="25640" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32240" yWindow="3500" windowWidth="25640" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBD_sequence_set" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="409">
   <si>
     <t>AncSarbecovirus_MAP</t>
   </si>
@@ -1193,42 +1193,6 @@
     <t>NITNLCPFGEVFNATTFPSVYAWERKRISNCVADYSVLYNST-SFSTFKCYGVSPTKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSTSGNYNYLYRLFRHGKLKPYERDISNVIYSPGGQSCS-AVGLNCYNPLKSYGFYTTSGVGYQPYRVVVLSFELLNAPATVCGPKLST</t>
   </si>
   <si>
-    <t>SARS2+Q498Y</t>
-  </si>
-  <si>
-    <t>SARS2+N501Y</t>
-  </si>
-  <si>
-    <t>SARS2+Q498Y+N501Y</t>
-  </si>
-  <si>
-    <t>SARS1+Y498Q</t>
-  </si>
-  <si>
-    <t>SARS1+T501Y</t>
-  </si>
-  <si>
-    <t>SARS1+Y498Q+T501Y</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSA-SFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTNGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSA-SFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFQPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSA-SFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNST-FFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCT-PPALNCYWPLNDYGFQTTTGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNST-FFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCT-PPALNCYWPLNDYGFYTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNST-FFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCT-PPALNCYWPLNDYGFQTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
-  </si>
-  <si>
     <t>PRD-0038+K493Y+T498W</t>
   </si>
   <si>
@@ -1262,24 +1226,6 @@
     <t>NITNLCPFGEVFNATTFPSVYAWERKRISNCVADYSVLYNSTSFSTFKCYGVSPTKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFTGCVLAWNTNSLDSSTSGNYNYLYRLFRHGKLKPYERDISNVIYSPGGQSCSAVGLNCYNPLKSYGFYTTSGVGYQPYRVVVLSFELLNAPATVCGPKLST</t>
   </si>
   <si>
-    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSASFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTNGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSASFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFQPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATRFASVYAWNRKRISNCVADYSVLYNSASFSTFKCYGVSPTKLNDLCFTNVYADSFVIRGDEVRQIAPGQTGKIADYNYKLPDDFTGCVIAWNSNNLDSKVGGNYNYLYRLFRKSNLKPFERDISTEIYQAGSTPCNGVEGFNCYFPLQSYGFYPTYGVGYQPYRVVVLSFELLHAPATVCGPKKST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNSTFFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCTPPALNCYWPLNDYGFQTTTGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNSTFFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCTPPALNCYWPLNDYGFYTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
-  </si>
-  <si>
-    <t>NITNLCPFGEVFNATKFPSVYAWERKKISNCVADYSVLYNSTFFSTFKCYGVSATKLNDLCFSNVYADSFVVKGDDVRQIAPGQTGVIADYNYKLPDDFMGCVLAWNTRNIDATSTGNYNYKYRYLRHGKLRPFERDISNVPFSPDGKPCTPPALNCYWPLNDYGFQTTYGIGYQPYRVVVLSFELLNAPATVCGPKLST</t>
-  </si>
-  <si>
     <t>AACATTACAAATCTATGTCCCTTCTCCGAGGTATTTAACGCTACCACATTCGCTAGTGTGTATGCTTGGAACAGGAAGCGTATTTCTAATTGTGTTGCCGATTACTCAGTCTTATACAACAGTACCTCATTCTCTACTTTTCAGTGTTATGGAGTCTCTTCTACAAAGCTTAACGACCTGTGCTTCACCAATGTGTACGCCGATTCCTTTGTTGTCAGGGGGGATGAGGTGCGTCAGATAGCACCAGGCCAAACGGGCGTTATAGCGGACTACAACTATAAGTTACCAGACGATTTTACCGGATGCGTCTTGGCGTGGAATTCAAGAAACCAAGACGCGAGTACCTCCGGGAACTTTAATTACTATTATCGTATCTGGAGAAGTGAAAAACTTCGTCCCTTTGAGAGGGACATCGCTCACTATGACTATCAAGTAGGGACCCAGTTTAAGTCTTCTCTTAAGAATTATGGATTCTATTCCAGCGCAGGGGACTCTCATCAACCGTACAGAGTAGTCGTACTAAGTTTCGAGTTATTGAACGCGCCTGCCACCGTTTGCGGTCCCAAACAGTCAACA</t>
   </si>
   <si>
@@ -1302,24 +1248,6 @@
   </si>
   <si>
     <t>AATATCACAAATTTGTGCCCGTTCGGAGAGGTTTTTAACGCTACCACGTTTCCTAGTGTTTACGCCTGGGAGAGGAAGAGAATTAGCAATTGTGTAGCCGATTACTCTGTGCTATACAACAGTACATCCTTTTCAACCTTCAAATGCTATGGTGTTAGCCCAACAAAACTGAACGATTTATGCTTCTCTAATGTCTATGCAGATTCTTTCGTGGTGAAAGGGGATGATGTTCGTCAAATCGCGCCGGGTCAAACTGGTGTGATAGCGGACTATAATTACAAGTTGCCGGATGATTTCACTGGTTGTGTTTTAGCATGGAACACGAACTCATTAGATTCCTCTACAAGCGGCAACTACAATTATCTGTATAGGTTATTCAGACACGGGAAACTGAAGCCGTATGAGAGGGACATCTCTAACGTCATCTACAGTCCTGGTGGACAATCATGTTCAGCCGTCGGGCTAAATTGTTACAATCCCCTGAAAAGCTATGGTTTCTATACAACAAGCGGTGTGGGCTATCAGCCCTACCGTGTTGTTGTCCTGTCCTTCGAATTATTAAATGCCCCTGCAACTGTATGCGGGCCTAAGCTATCCACG</t>
-  </si>
-  <si>
-    <t>AACATCACAAACCTATGTCCGTTTGGCGAGGTGTTTAATGCTACTAGGTTCGCAAGCGTTTACGCATGGAACCGTAAGAGAATCTCTAACTGCGTCGCAGATTATAGCGTTTTATATAACTCTGCTAGTTTTTCTACTTTTAAGTGTTACGGCGTGAGTCCTACGAAGTTGAACGATCTTTGCTTTACGAATGTGTACGCGGACAGCTTTGTCATCAGAGGTGATGAGGTAAGGCAGATAGCGCCCGGACAAACGGGGAAGATCGCAGACTACAATTATAAGCTGCCAGATGACTTTACCGGATGTGTGATTGCCTGGAACTCAAATAATCTGGACTCAAAGGTGGGTGGCAACTATAACTACCTGTATCGTCTTTTTAGGAAATCAAACTTAAAACCGTTTGAAAGGGACATATCCACTGAAATATATCAAGCGGGGAGCACACCGTGCAATGGCGTCGAGGGGTTTAACTGCTATTTCCCTCTACAGTCCTATGGGTTCTATCCTACTAATGGAGTTGGTTACCAACCCTATAGAGTGGTTGTTCTTAGTTTCGAGCTACTACATGCGCCAGCGACTGTGTGCGGCCCTAAGAAATCTACG</t>
-  </si>
-  <si>
-    <t>AATATCACGAACCTGTGTCCTTTTGGGGAGGTATTTAACGCCACCCGTTTCGCTTCAGTGTATGCCTGGAATAGAAAACGTATCAGCAATTGTGTCGCAGATTATTCAGTGCTATATAACTCCGCTAGTTTCTCTACGTTTAAGTGTTATGGCGTGTCCCCAACCAAGCTGAACGACCTGTGCTTTACAAACGTATATGCGGATTCATTTGTGATTAGAGGCGATGAAGTGAGACAAATTGCCCCAGGCCAGACCGGAAAGATTGCCGACTATAATTACAAACTGCCAGACGACTTTACGGGGTGTGTCATCGCTTGGAACAGCAACAATCTTGACAGTAAAGTTGGCGGGAACTATAATTATCTGTACCGTCTGTTCAGAAAAAGTAATCTTAAACCGTTTGAAAGGGACATCAGTACTGAGATTTATCAAGCGGGCTCAACCCCGTGTAATGGTGTAGAGGGGTTTAACTGCTATTTTCCACTACAATCCTACGGCTTCCAGCCAACGTACGGTGTGGGTTATCAACCCTATCGTGTCGTCGTATTGTCCTTCGAGCTATTACATGCTCCCGCGACCGTCTGTGGACCAAAGAAGTCCACC</t>
-  </si>
-  <si>
-    <t>AATATAACCAATCTGTGTCCCTTTGGAGAGGTTTTTAACGCTACGAGGTTCGCTTCTGTATATGCCTGGAACCGTAAGAGAATATCCAACTGTGTCGCTGACTACTCAGTTCTGTACAATTCTGCTAGTTTTAGCACCTTCAAGTGCTACGGAGTCAGCCCGACGAAGCTGAACGATTTGTGTTTTACGAATGTCTACGCTGACTCCTTCGTTATCAGGGGGGACGAAGTGAGGCAAATTGCTCCTGGCCAGACAGGGAAAATTGCTGATTATAATTACAAGTTACCGGATGATTTCACTGGATGCGTTATTGCATGGAACTCTAATAACCTTGATAGTAAGGTTGGCGGCAATTACAACTATTTGTACAGATTGTTCCGTAAGTCCAACCTGAAACCCTTCGAGAGAGATATTTCAACCGAAATTTACCAGGCAGGGTCCACGCCCTGCAATGGTGTAGAAGGGTTTAATTGCTATTTCCCGTTGCAGAGCTACGGATTCTACCCAACGTATGGAGTGGGTTATCAACCTTATCGTGTTGTCGTTTTGAGCTTTGAGCTGCTACATGCACCAGCAACTGTATGCGGGCCCAAGAAGTCTACT</t>
-  </si>
-  <si>
-    <t>AACATAACAAATTTGTGCCCTTTTGGAGAAGTTTTTAATGCAACAAAATTTCCATCCGTTTACGCATGGGAAAGAAAGAAAATCAGCAATTGTGTAGCCGATTACTCAGTACTTTACAATAGCACATTCTTTAGTACTTTCAAATGTTACGGGGTTTCAGCAACGAAATTAAACGATTTATGTTTCAGTAATGTGTATGCCGATAGTTTCGTCGTCAAAGGAGATGATGTGAGACAGATTGCACCCGGCCAGACTGGAGTTATTGCAGACTATAACTACAAACTACCAGACGATTTTATGGGATGTGTATTGGCATGGAACACGAGAAACATTGATGCTACGTCTACGGGTAACTATAACTATAAATATAGATACCTTAGGCACGGGAAGTTACGTCCGTTCGAGAGAGATATATCCAATGTACCATTTAGTCCTGATGGCAAGCCTTGCACTCCACCGGCCCTGAACTGTTATTGGCCCTTGAACGATTATGGTTTTCAAACAACTACGGGCATAGGTTACCAGCCATATAGGGTGGTAGTCCTGTCATTTGAGTTATTGAATGCGCCCGCTACGGTTTGCGGACCCAAACTGTCCACG</t>
-  </si>
-  <si>
-    <t>AATATAACAAACCTGTGTCCGTTTGGAGAAGTATTCAATGCTACTAAGTTCCCATCAGTTTACGCGTGGGAAAGGAAGAAGATTAGCAACTGTGTGGCAGACTACTCAGTGCTTTACAATAGCACCTTTTTCAGTACTTTCAAGTGCTATGGAGTAAGCGCCACTAAATTGAATGATTTATGTTTCTCAAACGTTTACGCAGATTCATTCGTGGTCAAAGGTGATGACGTGCGTCAGATAGCGCCAGGACAGACAGGAGTGATAGCGGACTATAACTACAAATTGCCGGACGATTTTATGGGCTGCGTCCTGGCATGGAATACGAGGAATATTGATGCAACCTCCACTGGCAACTATAACTATAAGTATCGTTACCTGAGGCACGGGAAACTAAGACCTTTCGAGAGAGACATATCAAATGTTCCATTTAGTCCAGACGGAAAGCCATGCACACCGCCAGCCCTTAACTGTTACTGGCCTCTAAATGACTATGGCTTTTATACAACGTATGGCATTGGTTATCAGCCGTACAGGGTAGTGGTCCTTAGCTTTGAGCTATTAAACGCTCCGGCTACGGTTTGCGGACCGAAACTGTCTACT</t>
-  </si>
-  <si>
-    <t>AATATCACCAACCTGTGTCCCTTCGGCGAGGTTTTCAACGCTACAAAATTCCCCTCCGTATATGCTTGGGAGAGAAAGAAGATCAGTAATTGCGTCGCAGACTATAGTGTTCTATATAATTCCACCTTCTTTAGCACTTTTAAGTGTTATGGAGTAAGTGCTACCAAACTTAATGATCTATGTTTCTCTAACGTGTACGCCGATTCTTTCGTTGTGAAAGGTGATGATGTTCGTCAGATTGCTCCTGGGCAAACGGGAGTGATTGCAGACTACAACTATAAGCTGCCGGACGATTTCATGGGCTGTGTATTAGCTTGGAATACCAGAAATATCGACGCCACATCAACTGGCAACTACAACTACAAATACAGATACTTACGTCATGGTAAACTGCGTCCTTTTGAGAGGGACATATCTAATGTGCCATTTTCTCCAGATGGAAAGCCCTGCACTCCGCCCGCGTTAAATTGCTATTGGCCACTTAACGACTACGGATTCCAGACAACGTACGGAATTGGCTATCAGCCGTATAGGGTGGTAGTGCTGAGCTTTGAGTTGTTAAATGCGCCTGCGACAGTGTGTGGGCCGAAATTAAGTACA</t>
   </si>
   <si>
     <t>RsYN04</t>
@@ -2205,11 +2133,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4751,24 +4679,50 @@
         <v>276</v>
       </c>
     </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>371</v>
+      </c>
+      <c r="C76">
+        <v>3001</v>
+      </c>
+      <c r="L76" t="s">
+        <v>398</v>
+      </c>
+      <c r="M76" t="s">
+        <v>389</v>
+      </c>
+      <c r="N76" t="s">
+        <v>372</v>
+      </c>
+      <c r="O76" t="s">
+        <v>275</v>
+      </c>
+      <c r="P76" t="s">
+        <v>276</v>
+      </c>
+    </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C77">
-        <v>3001</v>
+        <v>3002</v>
       </c>
       <c r="L77" t="s">
-        <v>416</v>
+        <v>399</v>
       </c>
       <c r="M77" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="N77" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="O77" t="s">
         <v>275</v>
@@ -4779,22 +4733,16 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>373</v>
-      </c>
-      <c r="C78">
-        <v>3002</v>
-      </c>
-      <c r="L78" t="s">
-        <v>417</v>
+        <v>375</v>
       </c>
       <c r="M78" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="N78" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="O78" t="s">
         <v>275</v>
@@ -4805,16 +4753,22 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>375</v>
+        <v>378</v>
+      </c>
+      <c r="C79">
+        <v>3003</v>
+      </c>
+      <c r="L79" t="s">
+        <v>400</v>
       </c>
       <c r="M79" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="N79" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="O79" t="s">
         <v>275</v>
@@ -4825,22 +4779,22 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C80">
-        <v>3003</v>
+        <v>3004</v>
       </c>
       <c r="L80" t="s">
-        <v>418</v>
+        <v>401</v>
       </c>
       <c r="M80" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="N80" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="O80" t="s">
         <v>275</v>
@@ -4851,22 +4805,22 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="C81">
-        <v>3004</v>
+        <v>3005</v>
       </c>
       <c r="L81" t="s">
-        <v>419</v>
+        <v>402</v>
       </c>
       <c r="M81" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="N81" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="O81" t="s">
         <v>275</v>
@@ -4877,22 +4831,22 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="C82">
-        <v>3005</v>
+        <v>3006</v>
       </c>
       <c r="L82" t="s">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="M82" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="N82" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="O82" t="s">
         <v>275</v>
@@ -4903,22 +4857,22 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C83">
-        <v>3006</v>
+        <v>3007</v>
       </c>
       <c r="L83" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="M83" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="N83" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="O83" t="s">
         <v>275</v>
@@ -4929,53 +4883,27 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C84">
-        <v>3007</v>
+        <v>3008</v>
       </c>
       <c r="L84" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="M84" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="N84" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="O84" t="s">
         <v>275</v>
       </c>
       <c r="P84" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>82</v>
-      </c>
-      <c r="B85" t="s">
-        <v>385</v>
-      </c>
-      <c r="C85">
-        <v>3008</v>
-      </c>
-      <c r="L85" t="s">
-        <v>423</v>
-      </c>
-      <c r="M85" t="s">
-        <v>409</v>
-      </c>
-      <c r="N85" t="s">
-        <v>386</v>
-      </c>
-      <c r="O85" t="s">
-        <v>275</v>
-      </c>
-      <c r="P85" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4984,174 +4912,18 @@
         <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>387</v>
-      </c>
-      <c r="C86">
-        <v>3009</v>
+        <v>406</v>
       </c>
       <c r="L86" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="M86" t="s">
-        <v>410</v>
-      </c>
-      <c r="N86" t="s">
-        <v>393</v>
+        <v>407</v>
       </c>
       <c r="O86" t="s">
         <v>275</v>
       </c>
       <c r="P86" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>84</v>
-      </c>
-      <c r="B87" t="s">
-        <v>388</v>
-      </c>
-      <c r="C87">
-        <v>3010</v>
-      </c>
-      <c r="L87" t="s">
-        <v>425</v>
-      </c>
-      <c r="M87" t="s">
-        <v>411</v>
-      </c>
-      <c r="N87" t="s">
-        <v>394</v>
-      </c>
-      <c r="O87" t="s">
-        <v>275</v>
-      </c>
-      <c r="P87" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>82</v>
-      </c>
-      <c r="B88" t="s">
-        <v>389</v>
-      </c>
-      <c r="C88">
-        <v>3011</v>
-      </c>
-      <c r="L88" t="s">
-        <v>426</v>
-      </c>
-      <c r="M88" t="s">
-        <v>412</v>
-      </c>
-      <c r="N88" t="s">
-        <v>395</v>
-      </c>
-      <c r="O88" t="s">
-        <v>275</v>
-      </c>
-      <c r="P88" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>86</v>
-      </c>
-      <c r="B89" t="s">
-        <v>390</v>
-      </c>
-      <c r="C89">
-        <v>3012</v>
-      </c>
-      <c r="L89" t="s">
-        <v>427</v>
-      </c>
-      <c r="M89" t="s">
-        <v>413</v>
-      </c>
-      <c r="N89" t="s">
-        <v>396</v>
-      </c>
-      <c r="O89" t="s">
-        <v>275</v>
-      </c>
-      <c r="P89" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>87</v>
-      </c>
-      <c r="B90" t="s">
-        <v>391</v>
-      </c>
-      <c r="C90">
-        <v>3013</v>
-      </c>
-      <c r="L90" t="s">
-        <v>428</v>
-      </c>
-      <c r="M90" t="s">
-        <v>414</v>
-      </c>
-      <c r="N90" t="s">
-        <v>397</v>
-      </c>
-      <c r="O90" t="s">
-        <v>275</v>
-      </c>
-      <c r="P90" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>88</v>
-      </c>
-      <c r="B91" t="s">
-        <v>392</v>
-      </c>
-      <c r="C91">
-        <v>3014</v>
-      </c>
-      <c r="L91" t="s">
-        <v>429</v>
-      </c>
-      <c r="M91" t="s">
-        <v>415</v>
-      </c>
-      <c r="N91" t="s">
-        <v>398</v>
-      </c>
-      <c r="O91" t="s">
-        <v>275</v>
-      </c>
-      <c r="P91" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>89</v>
-      </c>
-      <c r="B93" t="s">
-        <v>430</v>
-      </c>
-      <c r="L93" t="s">
-        <v>432</v>
-      </c>
-      <c r="M93" t="s">
-        <v>431</v>
-      </c>
-      <c r="O93" t="s">
-        <v>275</v>
-      </c>
-      <c r="P93" t="s">
         <v>276</v>
       </c>
     </row>

</xml_diff>